<commit_message>
Added tests for samples with aliases
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Sample_submission_v3_11_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Sample_submission_v3_11_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6415DC24-2918-DF47-A240-945FF20CFBA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751E8C52-5E31-4841-A6A4-0B35D5785438}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{A0A66DFA-CD12-4C05-A0E3-08B4F7BE356C}"/>
   </bookViews>
@@ -18,6 +18,9 @@
     <sheet name="Formulas" sheetId="3" r:id="rId3"/>
     <sheet name="tests" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_10x_Genomics_Dual_Index_NT_Series">Index!$X$2:$X$97</definedName>
     <definedName name="_10x_Genomics_scATAC">Index!$W$2:$W$97</definedName>
@@ -480,7 +483,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3508" uniqueCount="2931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3512" uniqueCount="2935">
   <si>
     <t>Alias</t>
   </si>
@@ -9307,12 +9310,24 @@
   <si>
     <t>MonsieurTest</t>
   </si>
+  <si>
+    <t>DNA1_Alias</t>
+  </si>
+  <si>
+    <t>RNA1_Alias</t>
+  </si>
+  <si>
+    <t>Blood1_Alias</t>
+  </si>
+  <si>
+    <t>Expectoration1_Alias</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9442,6 +9457,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -9576,7 +9598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9629,14 +9651,15 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9807,6 +9830,19 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Index"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10128,8 +10164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{316AE53C-2F5B-45FF-B158-B49E5DE33F91}">
   <dimension ref="A1:AE500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:N15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15"/>
@@ -10204,10 +10240,10 @@
       <c r="F6" s="25" t="s">
         <v>2901</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="29" t="s">
         <v>2898</v>
       </c>
-      <c r="I6" s="26"/>
+      <c r="I6" s="29"/>
       <c r="T6" s="25" t="s">
         <v>2901</v>
       </c>
@@ -10311,61 +10347,63 @@
       </c>
     </row>
     <row r="8" spans="1:30">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>2908</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="1" t="s">
+        <v>2931</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>2919</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="27" t="s">
         <v>2920</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="26" t="s">
         <v>58</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="27" t="s">
         <v>2916</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1">
         <v>9606</v>
       </c>
-      <c r="M8" s="28" t="s">
+      <c r="M8" s="27" t="s">
         <v>2918</v>
       </c>
-      <c r="N8" s="28" t="s">
+      <c r="N8" s="27" t="s">
         <v>2930</v>
       </c>
-      <c r="O8" s="28" t="s">
+      <c r="O8" s="27" t="s">
         <v>2917</v>
       </c>
-      <c r="P8" s="27" t="s">
+      <c r="P8" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="Q8" s="28" t="s">
+      <c r="Q8" s="27" t="s">
         <v>2918</v>
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
-      <c r="T8" s="29">
+      <c r="T8" s="28">
         <v>10</v>
       </c>
-      <c r="U8" s="29">
+      <c r="U8" s="28">
         <v>1</v>
       </c>
-      <c r="V8" s="29" t="s">
+      <c r="V8" s="28" t="s">
         <v>447</v>
       </c>
-      <c r="W8" s="28" t="s">
+      <c r="W8" s="27" t="s">
         <v>49</v>
       </c>
       <c r="X8" s="9"/>
@@ -10373,67 +10411,69 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
       <c r="AB8" s="9"/>
-      <c r="AC8" s="27" t="s">
+      <c r="AC8" s="26" t="s">
         <v>2927</v>
       </c>
-      <c r="AD8" s="28" t="s">
+      <c r="AD8" s="27" t="s">
         <v>2928</v>
       </c>
     </row>
     <row r="9" spans="1:30">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>2909</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="27" t="s">
+      <c r="C9" s="1" t="s">
+        <v>2932</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>2919</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>2920</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="27" t="s">
         <v>2916</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1">
         <v>9606</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="27" t="s">
         <v>2918</v>
       </c>
-      <c r="N9" s="28" t="s">
+      <c r="N9" s="27" t="s">
         <v>2930</v>
       </c>
-      <c r="O9" s="28" t="s">
+      <c r="O9" s="27" t="s">
         <v>2917</v>
       </c>
-      <c r="P9" s="27" t="s">
+      <c r="P9" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="Q9" s="28" t="s">
+      <c r="Q9" s="27" t="s">
         <v>2918</v>
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
-      <c r="T9" s="29">
+      <c r="T9" s="28">
         <v>20</v>
       </c>
       <c r="U9" s="9"/>
-      <c r="V9" s="29" t="s">
+      <c r="V9" s="28" t="s">
         <v>448</v>
       </c>
-      <c r="W9" s="28" t="s">
+      <c r="W9" s="27" t="s">
         <v>49</v>
       </c>
       <c r="X9" s="9"/>
@@ -10441,64 +10481,66 @@
       <c r="Z9" s="9"/>
       <c r="AA9" s="9"/>
       <c r="AB9" s="9"/>
-      <c r="AC9" s="27" t="s">
+      <c r="AC9" s="26" t="s">
         <v>2927</v>
       </c>
-      <c r="AD9" s="28" t="s">
+      <c r="AD9" s="27" t="s">
         <v>2928</v>
       </c>
     </row>
     <row r="10" spans="1:30">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>2910</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="30" t="s">
+        <v>2933</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>2921</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
         <v>2922</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="26" t="s">
         <v>58</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="27" t="s">
         <v>2916</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1">
         <v>9606</v>
       </c>
-      <c r="M10" s="28" t="s">
+      <c r="M10" s="27" t="s">
         <v>2918</v>
       </c>
-      <c r="N10" s="28" t="s">
+      <c r="N10" s="27" t="s">
         <v>2930</v>
       </c>
-      <c r="O10" s="28" t="s">
+      <c r="O10" s="27" t="s">
         <v>2917</v>
       </c>
-      <c r="P10" s="27" t="s">
+      <c r="P10" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="Q10" s="28" t="s">
+      <c r="Q10" s="27" t="s">
         <v>2918</v>
       </c>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
-      <c r="T10" s="29">
+      <c r="T10" s="28">
         <v>300</v>
       </c>
       <c r="U10" s="9"/>
-      <c r="V10" s="29" t="s">
+      <c r="V10" s="28" t="s">
         <v>448</v>
       </c>
       <c r="W10" s="9"/>
@@ -10507,64 +10549,66 @@
       <c r="Z10" s="9"/>
       <c r="AA10" s="9"/>
       <c r="AB10" s="9"/>
-      <c r="AC10" s="27" t="s">
+      <c r="AC10" s="26" t="s">
         <v>2927</v>
       </c>
-      <c r="AD10" s="28" t="s">
+      <c r="AD10" s="27" t="s">
         <v>2928</v>
       </c>
     </row>
     <row r="11" spans="1:30">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>2911</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="30" t="s">
+        <v>2934</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>2921</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="27" t="s">
         <v>2922</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="27" t="s">
         <v>2916</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1">
         <v>9606</v>
       </c>
-      <c r="M11" s="28" t="s">
+      <c r="M11" s="27" t="s">
         <v>2918</v>
       </c>
-      <c r="N11" s="28" t="s">
+      <c r="N11" s="27" t="s">
         <v>2930</v>
       </c>
-      <c r="O11" s="28" t="s">
+      <c r="O11" s="27" t="s">
         <v>2917</v>
       </c>
-      <c r="P11" s="27" t="s">
+      <c r="P11" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="Q11" s="28" t="s">
+      <c r="Q11" s="27" t="s">
         <v>2918</v>
       </c>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="29">
+      <c r="T11" s="28">
         <v>400</v>
       </c>
       <c r="U11" s="9"/>
-      <c r="V11" s="29" t="s">
+      <c r="V11" s="28" t="s">
         <v>448</v>
       </c>
       <c r="W11" s="9"/>
@@ -10573,64 +10617,64 @@
       <c r="Z11" s="9"/>
       <c r="AA11" s="9"/>
       <c r="AB11" s="9"/>
-      <c r="AC11" s="27" t="s">
+      <c r="AC11" s="26" t="s">
         <v>2927</v>
       </c>
-      <c r="AD11" s="28" t="s">
+      <c r="AD11" s="27" t="s">
         <v>2928</v>
       </c>
     </row>
     <row r="12" spans="1:30">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>2912</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="27" t="s">
         <v>2921</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="27" t="s">
         <v>2922</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="26" t="s">
         <v>60</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="27" t="s">
         <v>2916</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1">
         <v>9606</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="27" t="s">
         <v>2918</v>
       </c>
-      <c r="N12" s="28" t="s">
+      <c r="N12" s="27" t="s">
         <v>2930</v>
       </c>
-      <c r="O12" s="28" t="s">
+      <c r="O12" s="27" t="s">
         <v>2917</v>
       </c>
-      <c r="P12" s="27" t="s">
+      <c r="P12" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="Q12" s="28" t="s">
+      <c r="Q12" s="27" t="s">
         <v>2918</v>
       </c>
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
-      <c r="T12" s="29">
+      <c r="T12" s="28">
         <v>500</v>
       </c>
       <c r="U12" s="9"/>
-      <c r="V12" s="29" t="s">
+      <c r="V12" s="28" t="s">
         <v>448</v>
       </c>
       <c r="W12" s="9"/>
@@ -10639,64 +10683,64 @@
       <c r="Z12" s="9"/>
       <c r="AA12" s="9"/>
       <c r="AB12" s="9"/>
-      <c r="AC12" s="27" t="s">
+      <c r="AC12" s="26" t="s">
         <v>2927</v>
       </c>
-      <c r="AD12" s="28" t="s">
+      <c r="AD12" s="27" t="s">
         <v>2929</v>
       </c>
     </row>
     <row r="13" spans="1:30">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>2913</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>2921</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="27" t="s">
         <v>2922</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="26" t="s">
         <v>61</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="27" t="s">
         <v>2916</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1">
         <v>9606</v>
       </c>
-      <c r="M13" s="28" t="s">
+      <c r="M13" s="27" t="s">
         <v>2918</v>
       </c>
-      <c r="N13" s="28" t="s">
+      <c r="N13" s="27" t="s">
         <v>2930</v>
       </c>
-      <c r="O13" s="28" t="s">
+      <c r="O13" s="27" t="s">
         <v>2917</v>
       </c>
-      <c r="P13" s="27" t="s">
+      <c r="P13" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="Q13" s="28" t="s">
+      <c r="Q13" s="27" t="s">
         <v>2918</v>
       </c>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
-      <c r="T13" s="29">
+      <c r="T13" s="28">
         <v>600</v>
       </c>
       <c r="U13" s="9"/>
-      <c r="V13" s="29" t="s">
+      <c r="V13" s="28" t="s">
         <v>448</v>
       </c>
       <c r="W13" s="9"/>
@@ -10705,64 +10749,64 @@
       <c r="Z13" s="9"/>
       <c r="AA13" s="9"/>
       <c r="AB13" s="9"/>
-      <c r="AC13" s="27" t="s">
+      <c r="AC13" s="26" t="s">
         <v>2927</v>
       </c>
-      <c r="AD13" s="28" t="s">
+      <c r="AD13" s="27" t="s">
         <v>2929</v>
       </c>
     </row>
     <row r="14" spans="1:30">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>2914</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>2921</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="27" t="s">
         <v>2922</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="26" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="27" t="s">
         <v>2916</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1">
         <v>9606</v>
       </c>
-      <c r="M14" s="28" t="s">
+      <c r="M14" s="27" t="s">
         <v>2918</v>
       </c>
-      <c r="N14" s="28" t="s">
+      <c r="N14" s="27" t="s">
         <v>2930</v>
       </c>
-      <c r="O14" s="28" t="s">
+      <c r="O14" s="27" t="s">
         <v>2917</v>
       </c>
-      <c r="P14" s="27" t="s">
+      <c r="P14" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="Q14" s="28" t="s">
+      <c r="Q14" s="27" t="s">
         <v>2918</v>
       </c>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
-      <c r="T14" s="29">
+      <c r="T14" s="28">
         <v>70</v>
       </c>
       <c r="U14" s="9"/>
-      <c r="V14" s="29" t="s">
+      <c r="V14" s="28" t="s">
         <v>448</v>
       </c>
       <c r="W14" s="9"/>
@@ -10771,90 +10815,90 @@
       <c r="Z14" s="9"/>
       <c r="AA14" s="9"/>
       <c r="AB14" s="9"/>
-      <c r="AC14" s="27" t="s">
+      <c r="AC14" s="26" t="s">
         <v>2927</v>
       </c>
-      <c r="AD14" s="28" t="s">
+      <c r="AD14" s="27" t="s">
         <v>2929</v>
       </c>
     </row>
     <row r="15" spans="1:30">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>2915</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>2923</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="27" t="s">
         <v>2924</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="26" t="s">
         <v>58</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="27" t="s">
         <v>2916</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1">
         <v>9606</v>
       </c>
-      <c r="M15" s="28" t="s">
+      <c r="M15" s="27" t="s">
         <v>2918</v>
       </c>
-      <c r="N15" s="28" t="s">
+      <c r="N15" s="27" t="s">
         <v>2930</v>
       </c>
-      <c r="O15" s="28" t="s">
+      <c r="O15" s="27" t="s">
         <v>2917</v>
       </c>
-      <c r="P15" s="27" t="s">
+      <c r="P15" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="Q15" s="28" t="s">
+      <c r="Q15" s="27" t="s">
         <v>2918</v>
       </c>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
-      <c r="T15" s="29">
+      <c r="T15" s="28">
         <v>200</v>
       </c>
-      <c r="U15" s="29">
+      <c r="U15" s="28">
         <v>10</v>
       </c>
-      <c r="V15" s="28" t="s">
+      <c r="V15" s="27" t="s">
         <v>447</v>
       </c>
-      <c r="W15" s="28" t="s">
+      <c r="W15" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="X15" s="28" t="s">
+      <c r="X15" s="27" t="s">
         <v>450</v>
       </c>
-      <c r="Y15" s="28" t="s">
+      <c r="Y15" s="27" t="s">
         <v>451</v>
       </c>
-      <c r="Z15" s="28" t="s">
+      <c r="Z15" s="27" t="s">
         <v>456</v>
       </c>
-      <c r="AA15" s="28" t="s">
+      <c r="AA15" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="AB15" s="28" t="s">
+      <c r="AB15" s="27" t="s">
         <v>483</v>
       </c>
-      <c r="AC15" s="27" t="s">
+      <c r="AC15" s="26" t="s">
         <v>2925</v>
       </c>
-      <c r="AD15" s="28" t="s">
+      <c r="AD15" s="27" t="s">
         <v>2926</v>
       </c>
     </row>
@@ -26443,7 +26487,7 @@
   <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F34E8AE-82E2-4076-B67C-BDC8FE17713B}">
           <x14:formula1>
             <xm:f>Index!$A$2:$A$14</xm:f>
@@ -26496,43 +26540,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>W15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E09552E-1048-AA4D-8510-6184A005EB35}">
-          <x14:formula1>
-            <xm:f>[Sample_submission_v3_10_0.xlsx]Index!#REF!</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>AA15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{46082107-EBDA-2B44-AF15-2F444C0F076D}">
-          <x14:formula1>
-            <xm:f>[Sample_submission_v3_10_0.xlsx]Index!#REF!</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>Z15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{244E58B7-9629-3C49-BAA7-2BF75A99C3CD}">
-          <x14:formula1>
-            <xm:f>[Sample_submission_v3_10_0.xlsx]Index!#REF!</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>Y15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{972B612E-445C-DE43-AF0C-E27CE0A870DE}">
-          <x14:formula1>
-            <xm:f>[Sample_submission_v3_10_0.xlsx]Index!#REF!</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>X15</xm:sqref>
+          <xm:sqref>W15:AA15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>